<commit_message>
Add "Landscape-Insect Interations" to xlsx and update RMD.
</commit_message>
<xml_diff>
--- a/References/SEM SLR.xlsx
+++ b/References/SEM SLR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/emily_rampone_wsu_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R Projects\pathanalysismethods\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="323" documentId="8_{EEC48C55-1213-4483-AAB7-CCE24FCC63B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB820B68-8530-4320-AEC7-7A917221A1E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33360CB6-C583-4082-B9D7-912961BA8F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="525" windowWidth="25995" windowHeight="13905" xr2:uid="{15239279-75C0-4CDC-B78A-F1FB0EC56501}"/>
+    <workbookView xWindow="5610" yWindow="1283" windowWidth="21975" windowHeight="13410" activeTab="1" xr2:uid="{15239279-75C0-4CDC-B78A-F1FB0EC56501}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="127">
   <si>
     <t>Paper</t>
   </si>
@@ -854,7 +854,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -864,163 +864,163 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62477BFD-6FDE-4F8F-BFF9-07A571A997B0}">
   <dimension ref="B1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C31" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
         <v>112</v>
       </c>
@@ -1035,21 +1035,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E01CFE-976D-4763-954B-70A10A5D82BE}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.1328125" customWidth="1"/>
+    <col min="3" max="4" width="15.3984375" customWidth="1"/>
+    <col min="7" max="7" width="16.73046875" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" customWidth="1"/>
+    <col min="9" max="9" width="26.86328125" customWidth="1"/>
+    <col min="10" max="10" width="16.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1578,6 +1578,9 @@
       </c>
       <c r="H19" t="s">
         <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1594,13 +1597,13 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="102.42578125" customWidth="1"/>
+    <col min="2" max="2" width="102.3984375" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1799,10 +1802,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="K9" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D12" s="3" t="s">
         <v>115</v>
       </c>

</xml_diff>